<commit_message>
Split model.go to wind.go and itself
</commit_message>
<xml_diff>
--- a/Init_file.xlsx
+++ b/Init_file.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Total_High</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -53,6 +53,14 @@
   </si>
   <si>
     <t>Wind_w0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ground_rou</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -405,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -452,37 +460,34 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="B7">
-        <v>650</v>
-      </c>
-      <c r="C7">
-        <v>10</v>
+      <c r="C7" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B8">
-        <v>635</v>
+        <v>650</v>
       </c>
       <c r="C8">
         <v>10</v>
@@ -490,10 +495,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9">
-        <v>620</v>
+        <v>635</v>
       </c>
       <c r="C9">
         <v>10</v>
@@ -501,10 +506,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10">
-        <v>605</v>
+        <v>620</v>
       </c>
       <c r="C10">
         <v>10</v>
@@ -512,10 +517,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11">
-        <v>590</v>
+        <v>605</v>
       </c>
       <c r="C11">
         <v>10</v>
@@ -523,10 +528,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B12">
-        <v>575</v>
+        <v>590</v>
       </c>
       <c r="C12">
         <v>10</v>
@@ -534,10 +539,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13">
-        <v>560</v>
+        <v>575</v>
       </c>
       <c r="C13">
         <v>10</v>
@@ -545,10 +550,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B14">
-        <v>545</v>
+        <v>560</v>
       </c>
       <c r="C14">
         <v>10</v>
@@ -556,10 +561,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B15">
-        <v>530</v>
+        <v>545</v>
       </c>
       <c r="C15">
         <v>10</v>
@@ -567,10 +572,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B16">
-        <v>515</v>
+        <v>530</v>
       </c>
       <c r="C16">
         <v>10</v>
@@ -578,21 +583,21 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B17">
-        <v>500</v>
+        <v>515</v>
       </c>
       <c r="C17">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B18">
-        <v>485</v>
+        <v>500</v>
       </c>
       <c r="C18">
         <v>8</v>
@@ -600,10 +605,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B19">
-        <v>470</v>
+        <v>485</v>
       </c>
       <c r="C19">
         <v>8</v>
@@ -611,10 +616,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B20">
-        <v>455</v>
+        <v>470</v>
       </c>
       <c r="C20">
         <v>8</v>
@@ -622,10 +627,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B21">
-        <v>440</v>
+        <v>455</v>
       </c>
       <c r="C21">
         <v>8</v>
@@ -633,10 +638,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B22">
-        <v>425</v>
+        <v>440</v>
       </c>
       <c r="C22">
         <v>8</v>
@@ -644,10 +649,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B23">
-        <v>410</v>
+        <v>425</v>
       </c>
       <c r="C23">
         <v>8</v>
@@ -655,10 +660,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B24">
-        <v>395</v>
+        <v>410</v>
       </c>
       <c r="C24">
         <v>8</v>
@@ -666,10 +671,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B25">
-        <v>380</v>
+        <v>395</v>
       </c>
       <c r="C25">
         <v>8</v>
@@ -677,10 +682,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B26">
-        <v>365</v>
+        <v>380</v>
       </c>
       <c r="C26">
         <v>8</v>
@@ -688,10 +693,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A27">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B27">
-        <v>350</v>
+        <v>365</v>
       </c>
       <c r="C27">
         <v>8</v>
@@ -699,10 +704,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A28">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B28">
-        <v>335</v>
+        <v>350</v>
       </c>
       <c r="C28">
         <v>8</v>
@@ -710,10 +715,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A29">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B29">
-        <v>320</v>
+        <v>335</v>
       </c>
       <c r="C29">
         <v>8</v>
@@ -721,10 +726,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A30">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B30">
-        <v>305</v>
+        <v>320</v>
       </c>
       <c r="C30">
         <v>8</v>
@@ -732,10 +737,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A31">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B31">
-        <v>290</v>
+        <v>305</v>
       </c>
       <c r="C31">
         <v>8</v>
@@ -743,10 +748,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A32">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B32">
-        <v>275</v>
+        <v>290</v>
       </c>
       <c r="C32">
         <v>8</v>
@@ -754,10 +759,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A33">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B33">
-        <v>260</v>
+        <v>275</v>
       </c>
       <c r="C33">
         <v>8</v>
@@ -765,10 +770,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A34">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B34">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="C34">
         <v>8</v>
@@ -776,10 +781,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A35">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B35">
-        <v>230</v>
+        <v>245</v>
       </c>
       <c r="C35">
         <v>8</v>
@@ -787,10 +792,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A36">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B36">
-        <v>215</v>
+        <v>230</v>
       </c>
       <c r="C36">
         <v>8</v>
@@ -798,21 +803,21 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A37">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B37">
-        <v>200</v>
+        <v>215</v>
       </c>
       <c r="C37">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A38">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B38">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="C38">
         <v>6</v>
@@ -820,10 +825,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A39">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B39">
-        <v>170</v>
+        <v>185</v>
       </c>
       <c r="C39">
         <v>6</v>
@@ -831,10 +836,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A40">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B40">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="C40">
         <v>6</v>
@@ -842,12 +847,23 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A41">
+        <v>34</v>
+      </c>
+      <c r="B41">
+        <v>155</v>
+      </c>
+      <c r="C41">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A42">
         <v>35</v>
       </c>
-      <c r="B41">
+      <c r="B42">
         <v>140</v>
       </c>
-      <c r="C41">
+      <c r="C42">
         <v>6</v>
       </c>
     </row>

</xml_diff>